<commit_message>
Checks added, mock trial expanded
</commit_message>
<xml_diff>
--- a/src/MockTrialData.xlsx
+++ b/src/MockTrialData.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -101,9 +102,6 @@
     <t>Team15</t>
   </si>
   <si>
-    <t>Team61</t>
-  </si>
-  <si>
     <t>St. Bonaventure</t>
   </si>
   <si>
@@ -153,6 +151,9 @@
   </si>
   <si>
     <t>T16P1, T16P2, T16P3, T16P4, T16P5, T16P6</t>
+  </si>
+  <si>
+    <t>Team16</t>
   </si>
 </sst>
 </file>
@@ -473,9 +474,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -491,7 +490,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -502,7 +501,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -513,7 +512,7 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -524,7 +523,7 @@
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -535,7 +534,7 @@
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -546,7 +545,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -557,7 +556,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -568,7 +567,7 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -579,7 +578,7 @@
         <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -590,7 +589,7 @@
         <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -601,7 +600,7 @@
         <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -612,7 +611,7 @@
         <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -623,7 +622,7 @@
         <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -634,7 +633,7 @@
         <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -645,18 +644,18 @@
         <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" t="s">
         <v>25</v>
       </c>
-      <c r="B16" t="s">
-        <v>26</v>
-      </c>
       <c r="C16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>